<commit_message>
attaching export to admin page
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>שיוך</t>
   </si>
@@ -25,61 +25,55 @@
     <t>פרטי התקשרות</t>
   </si>
   <si>
+    <t>מיקוד</t>
+  </si>
+  <si>
+    <t>מס' אורחים שהוזמנו</t>
+  </si>
+  <si>
+    <t>קבוצה</t>
+  </si>
+  <si>
+    <t>טלפון רגיל</t>
+  </si>
+  <si>
+    <t>עיר</t>
+  </si>
+  <si>
+    <t>תא דואר</t>
+  </si>
+  <si>
+    <t>צד</t>
+  </si>
+  <si>
+    <t>אימייל</t>
+  </si>
+  <si>
+    <t>הזמנה לכבוד</t>
+  </si>
+  <si>
+    <t>אישרו שיגיעו</t>
+  </si>
+  <si>
     <t>צ'ק צפוי</t>
   </si>
   <si>
-    <t>עיר</t>
-  </si>
-  <si>
-    <t>מס' אורחים שהוזמנו</t>
-  </si>
-  <si>
-    <t>הזמנה לכבוד</t>
-  </si>
-  <si>
-    <t>צד</t>
-  </si>
-  <si>
-    <t>אימייל</t>
-  </si>
-  <si>
-    <t>אישרו שיגיעו</t>
-  </si>
-  <si>
-    <t>קבוצה</t>
-  </si>
-  <si>
-    <t>מיקוד</t>
-  </si>
-  <si>
-    <t>טלפון רגיל</t>
-  </si>
-  <si>
-    <t>תא דואר</t>
+    <t>רחוב</t>
   </si>
   <si>
     <t>סלולרי</t>
   </si>
   <si>
-    <t>רחוב</t>
+    <t>a and b</t>
   </si>
   <si>
     <t>חתן,כלה</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
     <t>פרסון ואורח\ת</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>a and b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Guest</t>
   </si>
 </sst>
 </file>
@@ -443,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,60 +470,60 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -540,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -557,81 +551,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
       <c r="M5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
         <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="M9" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>